<commit_message>
update reports with CODECOP 4.0.0, show complex PL/SQL units
</commit_message>
<xml_diff>
--- a/docs/tvdcc_report.xlsx
+++ b/docs/tvdcc_report.xlsx
@@ -21,7 +21,7 @@
   <definedNames>
     <definedName name="FilesTable">Files!$A$1:$O$116</definedName>
     <definedName name="IssuesTable">Issues!$A$1:$O$391</definedName>
-    <definedName name="UnitsTable">PLSQLUnits!$A$1:$H$1</definedName>
+    <definedName name="UnitsTable">PLSQLUnits!$A$1:$H$8</definedName>
   </definedNames>
   <calcPr calcId="140001"/>
   <pivotCaches>
@@ -1310,7 +1310,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -1479,7 +1479,7 @@
         </is>
       </c>
       <c r="B36" s="39" t="n">
-        <v>44287.75546296296</v>
+        <v>44287.835625</v>
       </c>
     </row>
     <row r="37">
@@ -1489,7 +1489,7 @@
         </is>
       </c>
       <c r="B37" s="40" t="n">
-        <v>44287.75560185185</v>
+        <v>44287.83577546296</v>
       </c>
     </row>
     <row r="38">
@@ -1499,7 +1499,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>9.637999999999995</v>
+        <v>10.031999999999998</v>
       </c>
     </row>
     <row r="39">
@@ -1882,6 +1882,279 @@
       </c>
       <c r="K1" s="21" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>guidelines/guideline_1040_04.sql</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>AnonymousPlsqlBlock</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>36.0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>29.0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="I2" s="43" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="J2" s="43" t="n">
+        <v>349.0333754971396</v>
+      </c>
+      <c r="K2" s="43" t="n">
+        <v>94.57346819440446</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>guidelines/guideline_4370_45.sql</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>AnonymousPlsqlBlock</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>27.0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="I3" s="43" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="J3" s="43" t="n">
+        <v>411.1982937621106</v>
+      </c>
+      <c r="K3" s="43" t="n">
+        <v>83.45140948052318</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>guidelines/guideline_4310_39.sql</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>my_package.password_check</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="I4" s="43" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="J4" s="43" t="n">
+        <v>491.54240635418904</v>
+      </c>
+      <c r="K4" s="43" t="n">
+        <v>86.13827722867563</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>guidelines/guideline_4310_39.sql</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>my_package.password_check</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>63.0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="I5" s="43" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="J5" s="43" t="n">
+        <v>491.54240635418904</v>
+      </c>
+      <c r="K5" s="43" t="n">
+        <v>86.13827722867563</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>guidelines/guideline_4320_40.sql</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>AnonymousPlsqlBlock</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="I6" s="43" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="J6" s="43" t="n">
+        <v>288.85263754543286</v>
+      </c>
+      <c r="K6" s="43" t="n">
+        <v>91.06596991130587</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>guidelines/guideline_4320_40.sql</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>AnonymousPlsqlBlock</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>41.0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>23.0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="I7" s="43" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="J7" s="43" t="n">
+        <v>346.1295543881475</v>
+      </c>
+      <c r="K7" s="43" t="n">
+        <v>86.66540775801556</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>guidelines/guideline_4370_45.sql</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>AnonymousPlsqlBlock</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>52.0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>23.0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="I8" s="43" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="J8" s="43" t="n">
+        <v>346.1295543881475</v>
+      </c>
+      <c r="K8" s="43" t="n">
+        <v>86.66540775801556</v>
       </c>
     </row>
   </sheetData>
@@ -2024,7 +2297,7 @@
         <v>221.0</v>
       </c>
       <c r="R2" s="45" t="n">
-        <v>0.027</v>
+        <v>0.031</v>
       </c>
     </row>
     <row r="3">
@@ -2140,7 +2413,7 @@
         <v>151.12938495797556</v>
       </c>
       <c r="R4" s="45" t="n">
-        <v>0.035</v>
+        <v>0.034</v>
       </c>
     </row>
     <row r="5">
@@ -2198,7 +2471,7 @@
         <v>115.83965560709328</v>
       </c>
       <c r="R5" s="45" t="n">
-        <v>0.043</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="6">
@@ -2314,7 +2587,7 @@
         <v>90.01136235652545</v>
       </c>
       <c r="R7" s="45" t="n">
-        <v>0.064</v>
+        <v>0.073</v>
       </c>
     </row>
     <row r="8">
@@ -2372,7 +2645,7 @@
         <v>109.6201354837433</v>
       </c>
       <c r="R8" s="45" t="n">
-        <v>0.028</v>
+        <v>0.036</v>
       </c>
     </row>
     <row r="9">
@@ -2430,7 +2703,7 @@
         <v>113.97978146648724</v>
       </c>
       <c r="R9" s="45" t="n">
-        <v>0.083</v>
+        <v>0.053</v>
       </c>
     </row>
     <row r="10">
@@ -2488,7 +2761,7 @@
         <v>99.38099733342473</v>
       </c>
       <c r="R10" s="45" t="n">
-        <v>0.037</v>
+        <v>0.057</v>
       </c>
     </row>
     <row r="11">
@@ -2546,7 +2819,7 @@
         <v>123.91518757305539</v>
       </c>
       <c r="R11" s="45" t="n">
-        <v>0.017</v>
+        <v>0.018</v>
       </c>
     </row>
     <row r="12">
@@ -2604,7 +2877,7 @@
         <v>221.0</v>
       </c>
       <c r="R12" s="45" t="n">
-        <v>0.02</v>
+        <v>0.021</v>
       </c>
     </row>
     <row r="13">
@@ -2662,7 +2935,7 @@
         <v>142.48477230839399</v>
       </c>
       <c r="R13" s="45" t="n">
-        <v>0.023</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="14">
@@ -2778,7 +3051,7 @@
         <v>221.0</v>
       </c>
       <c r="R15" s="45" t="n">
-        <v>0.018</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="16">
@@ -2836,7 +3109,7 @@
         <v>221.0</v>
       </c>
       <c r="R16" s="45" t="n">
-        <v>0.015</v>
+        <v>0.016</v>
       </c>
     </row>
     <row r="17">
@@ -2894,7 +3167,7 @@
         <v>221.0</v>
       </c>
       <c r="R17" s="45" t="n">
-        <v>0.032</v>
+        <v>0.035</v>
       </c>
     </row>
     <row r="18">
@@ -2952,7 +3225,7 @@
         <v>221.0</v>
       </c>
       <c r="R18" s="45" t="n">
-        <v>0.025</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="19">
@@ -3010,7 +3283,7 @@
         <v>95.29038288230932</v>
       </c>
       <c r="R19" s="45" t="n">
-        <v>0.047</v>
+        <v>0.052</v>
       </c>
     </row>
     <row r="20">
@@ -3068,7 +3341,7 @@
         <v>110.48163376087805</v>
       </c>
       <c r="R20" s="45" t="n">
-        <v>0.018</v>
+        <v>0.021</v>
       </c>
     </row>
     <row r="21">
@@ -3126,7 +3399,7 @@
         <v>108.91714839712569</v>
       </c>
       <c r="R21" s="45" t="n">
-        <v>0.022</v>
+        <v>0.025</v>
       </c>
     </row>
     <row r="22">
@@ -3184,7 +3457,7 @@
         <v>145.9099148782227</v>
       </c>
       <c r="R22" s="45" t="n">
-        <v>0.014</v>
+        <v>0.013</v>
       </c>
     </row>
     <row r="23">
@@ -3242,7 +3515,7 @@
         <v>103.94405539730502</v>
       </c>
       <c r="R23" s="45" t="n">
-        <v>0.065</v>
+        <v>0.083</v>
       </c>
     </row>
     <row r="24">
@@ -3300,7 +3573,7 @@
         <v>151.60914856804686</v>
       </c>
       <c r="R24" s="45" t="n">
-        <v>0.019</v>
+        <v>0.021</v>
       </c>
     </row>
     <row r="25">
@@ -3358,7 +3631,7 @@
         <v>152.30351180969438</v>
       </c>
       <c r="R25" s="45" t="n">
-        <v>0.015</v>
+        <v>0.021</v>
       </c>
     </row>
     <row r="26">
@@ -3416,7 +3689,7 @@
         <v>151.2237871128475</v>
       </c>
       <c r="R26" s="45" t="n">
-        <v>0.015</v>
+        <v>0.018</v>
       </c>
     </row>
     <row r="27">
@@ -3532,7 +3805,7 @@
         <v>123.8067241194785</v>
       </c>
       <c r="R28" s="45" t="n">
-        <v>0.024</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="29">
@@ -3590,7 +3863,7 @@
         <v>117.09300332586375</v>
       </c>
       <c r="R29" s="45" t="n">
-        <v>0.032</v>
+        <v>0.041</v>
       </c>
     </row>
     <row r="30">
@@ -3648,7 +3921,7 @@
         <v>91.35462766682645</v>
       </c>
       <c r="R30" s="45" t="n">
-        <v>0.03</v>
+        <v>0.035</v>
       </c>
     </row>
     <row r="31">
@@ -3706,7 +3979,7 @@
         <v>#NUM!</v>
       </c>
       <c r="R31" s="45" t="n">
-        <v>0.018</v>
+        <v>0.019</v>
       </c>
     </row>
     <row r="32">
@@ -3764,7 +4037,7 @@
         <v>118.27483045518112</v>
       </c>
       <c r="R32" s="45" t="n">
-        <v>0.019</v>
+        <v>0.025</v>
       </c>
     </row>
     <row r="33">
@@ -3822,7 +4095,7 @@
         <v>137.56479659118662</v>
       </c>
       <c r="R33" s="45" t="n">
-        <v>0.021</v>
+        <v>0.028</v>
       </c>
     </row>
     <row r="34">
@@ -3880,7 +4153,7 @@
         <v>133.30632238690072</v>
       </c>
       <c r="R34" s="45" t="n">
-        <v>0.017</v>
+        <v>0.018</v>
       </c>
     </row>
     <row r="35">
@@ -3938,7 +4211,7 @@
         <v>133.33855858920205</v>
       </c>
       <c r="R35" s="45" t="n">
-        <v>0.017</v>
+        <v>0.026</v>
       </c>
     </row>
     <row r="36">
@@ -3996,7 +4269,7 @@
         <v>132.21419842515994</v>
       </c>
       <c r="R36" s="45" t="n">
-        <v>0.015</v>
+        <v>0.018</v>
       </c>
     </row>
     <row r="37">
@@ -4054,7 +4327,7 @@
         <v>107.21170136233789</v>
       </c>
       <c r="R37" s="45" t="n">
-        <v>0.029</v>
+        <v>0.037</v>
       </c>
     </row>
     <row r="38">
@@ -4170,7 +4443,7 @@
         <v>110.48163376087805</v>
       </c>
       <c r="R39" s="45" t="n">
-        <v>0.024</v>
+        <v>0.026</v>
       </c>
     </row>
     <row r="40">
@@ -4228,7 +4501,7 @@
         <v>221.0</v>
       </c>
       <c r="R40" s="45" t="n">
-        <v>0.013</v>
+        <v>0.015</v>
       </c>
     </row>
     <row r="41">
@@ -4286,7 +4559,7 @@
         <v>139.07779353990418</v>
       </c>
       <c r="R41" s="45" t="n">
-        <v>0.018</v>
+        <v>0.019</v>
       </c>
     </row>
     <row r="42">
@@ -4402,7 +4675,7 @@
         <v>126.628315424</v>
       </c>
       <c r="R43" s="45" t="n">
-        <v>0.015</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="44">
@@ -4460,7 +4733,7 @@
         <v>153.19713314571302</v>
       </c>
       <c r="R44" s="45" t="n">
-        <v>0.016</v>
+        <v>0.019</v>
       </c>
     </row>
     <row r="45">
@@ -4518,7 +4791,7 @@
         <v>221.0</v>
       </c>
       <c r="R45" s="45" t="n">
-        <v>0.015</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="46">
@@ -4576,7 +4849,7 @@
         <v>110.73427596030683</v>
       </c>
       <c r="R46" s="45" t="n">
-        <v>0.022</v>
+        <v>0.024</v>
       </c>
     </row>
     <row r="47">
@@ -4634,7 +4907,7 @@
         <v>87.1489536992576</v>
       </c>
       <c r="R47" s="45" t="n">
-        <v>0.031</v>
+        <v>0.029</v>
       </c>
     </row>
     <row r="48">
@@ -4692,7 +4965,7 @@
         <v>#NUM!</v>
       </c>
       <c r="R48" s="45" t="n">
-        <v>0.014</v>
+        <v>0.017</v>
       </c>
     </row>
     <row r="49">
@@ -4750,7 +5023,7 @@
         <v>145.42961948150045</v>
       </c>
       <c r="R49" s="45" t="n">
-        <v>0.016</v>
+        <v>0.019</v>
       </c>
     </row>
     <row r="50">
@@ -4808,7 +5081,7 @@
         <v>150.35510587259904</v>
       </c>
       <c r="R50" s="45" t="n">
-        <v>0.016</v>
+        <v>0.015</v>
       </c>
     </row>
     <row r="51">
@@ -4982,7 +5255,7 @@
         <v>113.72759846562538</v>
       </c>
       <c r="R53" s="45" t="n">
-        <v>0.019</v>
+        <v>0.022</v>
       </c>
     </row>
     <row r="54">
@@ -5040,7 +5313,7 @@
         <v>139.9912104409607</v>
       </c>
       <c r="R54" s="45" t="n">
-        <v>1.921</v>
+        <v>1.846</v>
       </c>
     </row>
     <row r="55">
@@ -5098,7 +5371,7 @@
         <v>132.63771096485226</v>
       </c>
       <c r="R55" s="45" t="n">
-        <v>0.027</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="56">
@@ -5156,7 +5429,7 @@
         <v>112.08565495624394</v>
       </c>
       <c r="R56" s="45" t="n">
-        <v>0.076</v>
+        <v>0.097</v>
       </c>
     </row>
     <row r="57">
@@ -5272,7 +5545,7 @@
         <v>221.0</v>
       </c>
       <c r="R58" s="45" t="n">
-        <v>0.009</v>
+        <v>0.012</v>
       </c>
     </row>
     <row r="59">
@@ -5330,7 +5603,7 @@
         <v>132.91317102845775</v>
       </c>
       <c r="R59" s="45" t="n">
-        <v>0.017</v>
+        <v>0.021</v>
       </c>
     </row>
     <row r="60">
@@ -5388,7 +5661,7 @@
         <v>133.63803608961</v>
       </c>
       <c r="R60" s="45" t="n">
-        <v>0.023</v>
+        <v>0.031</v>
       </c>
     </row>
     <row r="61">
@@ -5446,7 +5719,7 @@
         <v>221.0</v>
       </c>
       <c r="R61" s="45" t="n">
-        <v>0.015</v>
+        <v>0.016</v>
       </c>
     </row>
     <row r="62">
@@ -5504,7 +5777,7 @@
         <v>221.0</v>
       </c>
       <c r="R62" s="45" t="n">
-        <v>0.017</v>
+        <v>0.029</v>
       </c>
     </row>
     <row r="63">
@@ -5562,7 +5835,7 @@
         <v>96.26919615452007</v>
       </c>
       <c r="R63" s="45" t="n">
-        <v>0.024</v>
+        <v>0.027</v>
       </c>
     </row>
     <row r="64">
@@ -5620,7 +5893,7 @@
         <v>104.29090470899365</v>
       </c>
       <c r="R64" s="45" t="n">
-        <v>0.024</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="65">
@@ -5678,7 +5951,7 @@
         <v>142.71816866484232</v>
       </c>
       <c r="R65" s="45" t="n">
-        <v>0.015</v>
+        <v>0.016</v>
       </c>
     </row>
     <row r="66">
@@ -5794,7 +6067,7 @@
         <v>105.68115152587492</v>
       </c>
       <c r="R67" s="45" t="n">
-        <v>0.027</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="68">
@@ -5852,7 +6125,7 @@
         <v>131.40077882702062</v>
       </c>
       <c r="R68" s="45" t="n">
-        <v>0.018</v>
+        <v>0.022</v>
       </c>
     </row>
     <row r="69">
@@ -5968,7 +6241,7 @@
         <v>116.5183576075469</v>
       </c>
       <c r="R70" s="45" t="n">
-        <v>0.03</v>
+        <v>0.031</v>
       </c>
     </row>
     <row r="71">
@@ -6026,7 +6299,7 @@
         <v>105.26154228636585</v>
       </c>
       <c r="R71" s="45" t="n">
-        <v>0.034</v>
+        <v>0.044</v>
       </c>
     </row>
     <row r="72">
@@ -6084,7 +6357,7 @@
         <v>166.00720689569917</v>
       </c>
       <c r="R72" s="45" t="n">
-        <v>0.026</v>
+        <v>0.049</v>
       </c>
     </row>
     <row r="73">
@@ -6142,7 +6415,7 @@
         <v>115.50706853078891</v>
       </c>
       <c r="R73" s="45" t="n">
-        <v>0.026</v>
+        <v>0.036</v>
       </c>
     </row>
     <row r="74">
@@ -6200,7 +6473,7 @@
         <v>143.80142955442838</v>
       </c>
       <c r="R74" s="45" t="n">
-        <v>0.021</v>
+        <v>0.036</v>
       </c>
     </row>
     <row r="75">
@@ -6258,7 +6531,7 @@
         <v>145.59474755786417</v>
       </c>
       <c r="R75" s="45" t="n">
-        <v>0.02</v>
+        <v>0.028</v>
       </c>
     </row>
     <row r="76">
@@ -6316,7 +6589,7 @@
         <v>140.4656198011365</v>
       </c>
       <c r="R76" s="45" t="n">
-        <v>0.016</v>
+        <v>0.017</v>
       </c>
     </row>
     <row r="77">
@@ -6374,7 +6647,7 @@
         <v>132.50090567781749</v>
       </c>
       <c r="R77" s="45" t="n">
-        <v>0.018</v>
+        <v>0.019</v>
       </c>
     </row>
     <row r="78">
@@ -6432,7 +6705,7 @@
         <v>118.81585552012493</v>
       </c>
       <c r="R78" s="45" t="n">
-        <v>0.022</v>
+        <v>0.025</v>
       </c>
     </row>
     <row r="79">
@@ -6490,7 +6763,7 @@
         <v>106.67823290037101</v>
       </c>
       <c r="R79" s="45" t="n">
-        <v>0.036</v>
+        <v>0.037</v>
       </c>
     </row>
     <row r="80">
@@ -6548,7 +6821,7 @@
         <v>131.19036647187858</v>
       </c>
       <c r="R80" s="45" t="n">
-        <v>0.021</v>
+        <v>0.022</v>
       </c>
     </row>
     <row r="81">
@@ -6664,7 +6937,7 @@
         <v>221.0</v>
       </c>
       <c r="R82" s="45" t="n">
-        <v>0.012</v>
+        <v>0.013</v>
       </c>
     </row>
     <row r="83">
@@ -6722,7 +6995,7 @@
         <v>221.0</v>
       </c>
       <c r="R83" s="45" t="n">
-        <v>0.012</v>
+        <v>0.014</v>
       </c>
     </row>
     <row r="84">
@@ -6780,7 +7053,7 @@
         <v>125.3444896167396</v>
       </c>
       <c r="R84" s="45" t="n">
-        <v>0.024</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="85">
@@ -6838,7 +7111,7 @@
         <v>221.0</v>
       </c>
       <c r="R85" s="45" t="n">
-        <v>0.041</v>
+        <v>0.051</v>
       </c>
     </row>
     <row r="86">
@@ -6896,7 +7169,7 @@
         <v>149.5981155846649</v>
       </c>
       <c r="R86" s="45" t="n">
-        <v>0.031</v>
+        <v>0.038</v>
       </c>
     </row>
     <row r="87">
@@ -6954,7 +7227,7 @@
         <v>117.63573797074517</v>
       </c>
       <c r="R87" s="45" t="n">
-        <v>0.028</v>
+        <v>0.035</v>
       </c>
     </row>
     <row r="88">
@@ -7012,7 +7285,7 @@
         <v>107.62988220575821</v>
       </c>
       <c r="R88" s="45" t="n">
-        <v>0.046</v>
+        <v>0.034</v>
       </c>
     </row>
     <row r="89">
@@ -7070,7 +7343,7 @@
         <v>99.66960507086627</v>
       </c>
       <c r="R89" s="45" t="n">
-        <v>0.042</v>
+        <v>0.052</v>
       </c>
     </row>
     <row r="90">
@@ -7128,7 +7401,7 @@
         <v>109.5421618642685</v>
       </c>
       <c r="R90" s="45" t="n">
-        <v>0.018</v>
+        <v>0.021</v>
       </c>
     </row>
     <row r="91">
@@ -7186,7 +7459,7 @@
         <v>221.0</v>
       </c>
       <c r="R91" s="45" t="n">
-        <v>0.014</v>
+        <v>0.016</v>
       </c>
     </row>
     <row r="92">
@@ -7244,7 +7517,7 @@
         <v>221.0</v>
       </c>
       <c r="R92" s="45" t="n">
-        <v>0.014</v>
+        <v>0.016</v>
       </c>
     </row>
     <row r="93">
@@ -7302,7 +7575,7 @@
         <v>127.63887698102158</v>
       </c>
       <c r="R93" s="45" t="n">
-        <v>0.015</v>
+        <v>0.016</v>
       </c>
     </row>
     <row r="94">
@@ -7360,7 +7633,7 @@
         <v>113.86381995730078</v>
       </c>
       <c r="R94" s="45" t="n">
-        <v>0.019</v>
+        <v>0.023</v>
       </c>
     </row>
     <row r="95">
@@ -7418,7 +7691,7 @@
         <v>109.15334102472441</v>
       </c>
       <c r="R95" s="45" t="n">
-        <v>0.023</v>
+        <v>0.026</v>
       </c>
     </row>
     <row r="96">
@@ -7476,7 +7749,7 @@
         <v>118.37999486566261</v>
       </c>
       <c r="R96" s="45" t="n">
-        <v>0.024</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="97">
@@ -7592,7 +7865,7 @@
         <v>109.44604437955596</v>
       </c>
       <c r="R98" s="45" t="n">
-        <v>0.018</v>
+        <v>0.022</v>
       </c>
     </row>
     <row r="99">
@@ -7650,7 +7923,7 @@
         <v>123.45145111688797</v>
       </c>
       <c r="R99" s="45" t="n">
-        <v>0.017</v>
+        <v>0.023</v>
       </c>
     </row>
     <row r="100">
@@ -7708,7 +7981,7 @@
         <v>110.84961935738808</v>
       </c>
       <c r="R100" s="45" t="n">
-        <v>0.022</v>
+        <v>0.021</v>
       </c>
     </row>
     <row r="101">
@@ -7766,7 +8039,7 @@
         <v>173.02559348033859</v>
       </c>
       <c r="R101" s="45" t="n">
-        <v>0.014</v>
+        <v>0.017</v>
       </c>
     </row>
     <row r="102">
@@ -7824,7 +8097,7 @@
         <v>115.5196055428162</v>
       </c>
       <c r="R102" s="45" t="n">
-        <v>0.017</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="103">
@@ -7882,7 +8155,7 @@
         <v>#NUM!</v>
       </c>
       <c r="R103" s="45" t="n">
-        <v>0.012</v>
+        <v>0.016</v>
       </c>
     </row>
     <row r="104">
@@ -7940,7 +8213,7 @@
         <v>#NUM!</v>
       </c>
       <c r="R104" s="45" t="n">
-        <v>0.011</v>
+        <v>0.015</v>
       </c>
     </row>
     <row r="105">
@@ -7998,7 +8271,7 @@
         <v>221.0</v>
       </c>
       <c r="R105" s="45" t="n">
-        <v>5.129</v>
+        <v>5.227</v>
       </c>
     </row>
     <row r="106">
@@ -8056,7 +8329,7 @@
         <v>221.0</v>
       </c>
       <c r="R106" s="45" t="n">
-        <v>0.015</v>
+        <v>0.014</v>
       </c>
     </row>
     <row r="107">
@@ -8114,7 +8387,7 @@
         <v>114.54162457205497</v>
       </c>
       <c r="R107" s="45" t="n">
-        <v>0.023</v>
+        <v>0.017</v>
       </c>
     </row>
     <row r="108">
@@ -8230,7 +8503,7 @@
         <v>140.48917406104826</v>
       </c>
       <c r="R109" s="45" t="n">
-        <v>0.015</v>
+        <v>0.013</v>
       </c>
     </row>
     <row r="110">
@@ -8346,7 +8619,7 @@
         <v>104.21133318296063</v>
       </c>
       <c r="R111" s="45" t="n">
-        <v>0.024</v>
+        <v>0.027</v>
       </c>
     </row>
     <row r="112">
@@ -8404,7 +8677,7 @@
         <v>111.54832912385558</v>
       </c>
       <c r="R112" s="45" t="n">
-        <v>0.017</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="113">
@@ -8462,7 +8735,7 @@
         <v>221.0</v>
       </c>
       <c r="R113" s="45" t="n">
-        <v>0.015</v>
+        <v>0.016</v>
       </c>
     </row>
     <row r="114">
@@ -8578,7 +8851,7 @@
         <v>110.07988968628534</v>
       </c>
       <c r="R115" s="45" t="n">
-        <v>0.024</v>
+        <v>0.032</v>
       </c>
     </row>
     <row r="116">

</xml_diff>

<commit_message>
updated reports with complexity=4 to show show complex units
</commit_message>
<xml_diff>
--- a/docs/tvdcc_report.xlsx
+++ b/docs/tvdcc_report.xlsx
@@ -21,7 +21,7 @@
   <definedNames>
     <definedName name="FilesTable">Files!$A$1:$O$123</definedName>
     <definedName name="IssuesTable">Issues!$A$1:$O$299</definedName>
-    <definedName name="UnitsTable">PLSQLUnits!$A$1:$H$1</definedName>
+    <definedName name="UnitsTable">PLSQLUnits!$A$1:$H$8</definedName>
   </definedNames>
   <calcPr calcId="140001"/>
   <pivotCaches>
@@ -1310,7 +1310,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -1479,7 +1479,7 @@
         </is>
       </c>
       <c r="B36" s="39" t="n">
-        <v>44806.47466435185</v>
+        <v>44806.49607638889</v>
       </c>
     </row>
     <row r="37">
@@ -1489,7 +1489,7 @@
         </is>
       </c>
       <c r="B37" s="40" t="n">
-        <v>44806.4747337963</v>
+        <v>44806.496145833335</v>
       </c>
     </row>
     <row r="38">
@@ -1499,7 +1499,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>5.761</v>
+        <v>5.768</v>
       </c>
     </row>
     <row r="39">
@@ -1882,6 +1882,279 @@
       </c>
       <c r="K1" s="21" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>guidelines/guideline_1040_04.sql</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>AnonymousPlsqlBlock</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>31.0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>31.0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="I2" s="43" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="J2" s="43" t="n">
+        <v>349.0333754971396</v>
+      </c>
+      <c r="K2" s="43" t="n">
+        <v>93.3400232177323</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>guidelines/guideline_4370_45.sql</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>AnonymousPlsqlBlock</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>29.0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>29.0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="I3" s="43" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="J3" s="43" t="n">
+        <v>411.1982937621106</v>
+      </c>
+      <c r="K3" s="43" t="n">
+        <v>82.40588543809453</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>guidelines/guideline_4310_39.sql</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>my_package.password_check</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="I4" s="43" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="J4" s="43" t="n">
+        <v>491.54240635418904</v>
+      </c>
+      <c r="K4" s="43" t="n">
+        <v>86.13827722867563</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>guidelines/guideline_4310_39.sql</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>my_package.password_check</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>63.0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="I5" s="43" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="J5" s="43" t="n">
+        <v>491.54240635418904</v>
+      </c>
+      <c r="K5" s="43" t="n">
+        <v>86.13827722867563</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>guidelines/guideline_4320_40.sql</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>AnonymousPlsqlBlock</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="I6" s="43" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="J6" s="43" t="n">
+        <v>288.85263754543286</v>
+      </c>
+      <c r="K6" s="43" t="n">
+        <v>91.06596991130587</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>guidelines/guideline_4320_40.sql</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>AnonymousPlsqlBlock</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>41.0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="I7" s="43" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="J7" s="43" t="n">
+        <v>346.1295543881475</v>
+      </c>
+      <c r="K7" s="43" t="n">
+        <v>85.46485860912527</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>guidelines/guideline_4370_45.sql</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>AnonymousPlsqlBlock</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>54.0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="I8" s="43" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="J8" s="43" t="n">
+        <v>346.1295543881475</v>
+      </c>
+      <c r="K8" s="43" t="n">
+        <v>85.46485860912527</v>
       </c>
     </row>
   </sheetData>
@@ -2024,7 +2297,7 @@
         <v>108.79331316511838</v>
       </c>
       <c r="R2" s="45" t="n">
-        <v>0.01</v>
+        <v>0.008</v>
       </c>
     </row>
     <row r="3">
@@ -2082,7 +2355,7 @@
         <v>134.43440892942934</v>
       </c>
       <c r="R3" s="45" t="n">
-        <v>0.011</v>
+        <v>0.008</v>
       </c>
     </row>
     <row r="4">
@@ -2140,7 +2413,7 @@
         <v>103.94405539730502</v>
       </c>
       <c r="R4" s="45" t="n">
-        <v>0.044</v>
+        <v>0.034</v>
       </c>
     </row>
     <row r="5">
@@ -2198,7 +2471,7 @@
         <v>147.13565074292492</v>
       </c>
       <c r="R5" s="45" t="n">
-        <v>0.015</v>
+        <v>0.017</v>
       </c>
     </row>
     <row r="6">
@@ -2256,7 +2529,7 @@
         <v>96.19335468818096</v>
       </c>
       <c r="R6" s="45" t="n">
-        <v>0.017</v>
+        <v>0.067</v>
       </c>
     </row>
     <row r="7">
@@ -2314,7 +2587,7 @@
         <v>90.58449796027804</v>
       </c>
       <c r="R7" s="45" t="n">
-        <v>0.028</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="8">
@@ -2372,7 +2645,7 @@
         <v>111.19442190059088</v>
       </c>
       <c r="R8" s="45" t="n">
-        <v>0.012</v>
+        <v>0.011</v>
       </c>
     </row>
     <row r="9">
@@ -2430,7 +2703,7 @@
         <v>113.92738721160785</v>
       </c>
       <c r="R9" s="45" t="n">
-        <v>0.019</v>
+        <v>0.013</v>
       </c>
     </row>
     <row r="10">
@@ -2488,7 +2761,7 @@
         <v>133.98544329794808</v>
       </c>
       <c r="R10" s="45" t="n">
-        <v>0.019</v>
+        <v>0.011</v>
       </c>
     </row>
     <row r="11">
@@ -2546,7 +2819,7 @@
         <v>133.086042916232</v>
       </c>
       <c r="R11" s="45" t="n">
-        <v>0.008</v>
+        <v>0.006</v>
       </c>
     </row>
     <row r="12">
@@ -2604,7 +2877,7 @@
         <v>133.61523810185807</v>
       </c>
       <c r="R12" s="45" t="n">
-        <v>0.007</v>
+        <v>0.013</v>
       </c>
     </row>
     <row r="13">
@@ -2720,7 +2993,7 @@
         <v>221.0</v>
       </c>
       <c r="R14" s="45" t="n">
-        <v>0.058</v>
+        <v>0.009</v>
       </c>
     </row>
     <row r="15">
@@ -2778,7 +3051,7 @@
         <v>85.93467540385956</v>
       </c>
       <c r="R15" s="45" t="n">
-        <v>0.013</v>
+        <v>0.011</v>
       </c>
     </row>
     <row r="16">
@@ -2894,7 +3167,7 @@
         <v>125.47722639453002</v>
       </c>
       <c r="R17" s="45" t="n">
-        <v>0.008</v>
+        <v>0.011</v>
       </c>
     </row>
     <row r="18">
@@ -2952,7 +3225,7 @@
         <v>126.29271511408461</v>
       </c>
       <c r="R18" s="45" t="n">
-        <v>0.013</v>
+        <v>0.009</v>
       </c>
     </row>
     <row r="19">
@@ -3010,7 +3283,7 @@
         <v>126.628315424</v>
       </c>
       <c r="R19" s="45" t="n">
-        <v>0.009</v>
+        <v>0.008</v>
       </c>
     </row>
     <row r="20">
@@ -3068,7 +3341,7 @@
         <v>117.09300332586375</v>
       </c>
       <c r="R20" s="45" t="n">
-        <v>0.06</v>
+        <v>0.057</v>
       </c>
     </row>
     <row r="21">
@@ -3126,7 +3399,7 @@
         <v>137.56479659118662</v>
       </c>
       <c r="R21" s="45" t="n">
-        <v>0.008</v>
+        <v>0.009</v>
       </c>
     </row>
     <row r="22">
@@ -3300,7 +3573,7 @@
         <v>123.91518757305539</v>
       </c>
       <c r="R24" s="45" t="n">
-        <v>0.008</v>
+        <v>0.007</v>
       </c>
     </row>
     <row r="25">
@@ -3358,7 +3631,7 @@
         <v>125.3444896167396</v>
       </c>
       <c r="R25" s="45" t="n">
-        <v>0.011</v>
+        <v>0.013</v>
       </c>
     </row>
     <row r="26">
@@ -3416,7 +3689,7 @@
         <v>221.0</v>
       </c>
       <c r="R26" s="45" t="n">
-        <v>0.012</v>
+        <v>0.013</v>
       </c>
     </row>
     <row r="27">
@@ -3474,7 +3747,7 @@
         <v>110.48163376087805</v>
       </c>
       <c r="R27" s="45" t="n">
-        <v>0.052</v>
+        <v>0.048</v>
       </c>
     </row>
     <row r="28">
@@ -3590,7 +3863,7 @@
         <v>221.0</v>
       </c>
       <c r="R29" s="45" t="n">
-        <v>0.006</v>
+        <v>0.007</v>
       </c>
     </row>
     <row r="30">
@@ -3706,7 +3979,7 @@
         <v>221.0</v>
       </c>
       <c r="R31" s="45" t="n">
-        <v>0.008</v>
+        <v>0.007</v>
       </c>
     </row>
     <row r="32">
@@ -3822,7 +4095,7 @@
         <v>110.73427596030683</v>
       </c>
       <c r="R33" s="45" t="n">
-        <v>0.059</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="34">
@@ -3880,7 +4153,7 @@
         <v>123.8067241194785</v>
       </c>
       <c r="R34" s="45" t="n">
-        <v>0.013</v>
+        <v>0.012</v>
       </c>
     </row>
     <row r="35">
@@ -3938,7 +4211,7 @@
         <v>123.451451116888</v>
       </c>
       <c r="R35" s="45" t="n">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="36">
@@ -3996,7 +4269,7 @@
         <v>116.14843422251893</v>
       </c>
       <c r="R36" s="45" t="n">
-        <v>0.007</v>
+        <v>0.008</v>
       </c>
     </row>
     <row r="37">
@@ -4054,7 +4327,7 @@
         <v>110.48163376087805</v>
       </c>
       <c r="R37" s="45" t="n">
-        <v>0.009</v>
+        <v>0.008</v>
       </c>
     </row>
     <row r="38">
@@ -4112,7 +4385,7 @@
         <v>142.9264720534504</v>
       </c>
       <c r="R38" s="45" t="n">
-        <v>0.012</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="39">
@@ -4170,7 +4443,7 @@
         <v>131.67694991865315</v>
       </c>
       <c r="R39" s="45" t="n">
-        <v>0.011</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="40">
@@ -4286,7 +4559,7 @@
         <v>132.63771096485226</v>
       </c>
       <c r="R41" s="45" t="n">
-        <v>0.03</v>
+        <v>0.028</v>
       </c>
     </row>
     <row r="42">
@@ -4344,7 +4617,7 @@
         <v>108.64189755804611</v>
       </c>
       <c r="R42" s="45" t="n">
-        <v>0.032</v>
+        <v>0.033</v>
       </c>
     </row>
     <row r="43">
@@ -4402,7 +4675,7 @@
         <v>221.0</v>
       </c>
       <c r="R43" s="45" t="n">
-        <v>0.049</v>
+        <v>0.052</v>
       </c>
     </row>
     <row r="44">
@@ -4460,7 +4733,7 @@
         <v>127.14835544286512</v>
       </c>
       <c r="R44" s="45" t="n">
-        <v>0.057</v>
+        <v>0.012</v>
       </c>
     </row>
     <row r="45">
@@ -4518,7 +4791,7 @@
         <v>152.30351180969438</v>
       </c>
       <c r="R45" s="45" t="n">
-        <v>0.054</v>
+        <v>0.057</v>
       </c>
     </row>
     <row r="46">
@@ -4634,7 +4907,7 @@
         <v>151.2237871128475</v>
       </c>
       <c r="R47" s="45" t="n">
-        <v>0.007</v>
+        <v>0.059</v>
       </c>
     </row>
     <row r="48">
@@ -4692,7 +4965,7 @@
         <v>133.63803608961</v>
       </c>
       <c r="R48" s="45" t="n">
-        <v>0.014</v>
+        <v>0.012</v>
       </c>
     </row>
     <row r="49">
@@ -4750,7 +5023,7 @@
         <v>221.0</v>
       </c>
       <c r="R49" s="45" t="n">
-        <v>0.011</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="50">
@@ -4808,7 +5081,7 @@
         <v>221.0</v>
       </c>
       <c r="R50" s="45" t="n">
-        <v>0.01</v>
+        <v>0.008</v>
       </c>
     </row>
     <row r="51">
@@ -4866,7 +5139,7 @@
         <v>221.0</v>
       </c>
       <c r="R51" s="45" t="n">
-        <v>0.052</v>
+        <v>0.054</v>
       </c>
     </row>
     <row r="52">
@@ -4924,7 +5197,7 @@
         <v>109.44604437955596</v>
       </c>
       <c r="R52" s="45" t="n">
-        <v>0.049</v>
+        <v>0.048</v>
       </c>
     </row>
     <row r="53">
@@ -4982,7 +5255,7 @@
         <v>94.22550780764529</v>
       </c>
       <c r="R53" s="45" t="n">
-        <v>0.022</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="54">
@@ -5040,7 +5313,7 @@
         <v>104.29090470899365</v>
       </c>
       <c r="R54" s="45" t="n">
-        <v>0.009</v>
+        <v>0.008</v>
       </c>
     </row>
     <row r="55">
@@ -5098,7 +5371,7 @@
         <v>138.9520445186466</v>
       </c>
       <c r="R55" s="45" t="n">
-        <v>0.008</v>
+        <v>0.006</v>
       </c>
     </row>
     <row r="56">
@@ -5156,7 +5429,7 @@
         <v>115.83965560709328</v>
       </c>
       <c r="R56" s="45" t="n">
-        <v>0.014</v>
+        <v>0.017</v>
       </c>
     </row>
     <row r="57">
@@ -5214,7 +5487,7 @@
         <v>101.96914373639542</v>
       </c>
       <c r="R57" s="45" t="n">
-        <v>0.01</v>
+        <v>0.009</v>
       </c>
     </row>
     <row r="58">
@@ -5330,7 +5603,7 @@
         <v>135.85166593632852</v>
       </c>
       <c r="R59" s="45" t="n">
-        <v>0.007</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="60">
@@ -5388,7 +5661,7 @@
         <v>117.81580773941356</v>
       </c>
       <c r="R60" s="45" t="n">
-        <v>0.008</v>
+        <v>0.007</v>
       </c>
     </row>
     <row r="61">
@@ -5446,7 +5719,7 @@
         <v>113.99239390172157</v>
       </c>
       <c r="R61" s="45" t="n">
-        <v>0.011</v>
+        <v>0.012</v>
       </c>
     </row>
     <row r="62">
@@ -5504,7 +5777,7 @@
         <v>139.9912104409607</v>
       </c>
       <c r="R62" s="45" t="n">
-        <v>0.462</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="63">
@@ -5562,7 +5835,7 @@
         <v>158.4661119261645</v>
       </c>
       <c r="R63" s="45" t="n">
-        <v>0.015</v>
+        <v>0.014</v>
       </c>
     </row>
     <row r="64">
@@ -5620,7 +5893,7 @@
         <v>221.0</v>
       </c>
       <c r="R64" s="45" t="n">
-        <v>0.025</v>
+        <v>0.028</v>
       </c>
     </row>
     <row r="65">
@@ -5678,7 +5951,7 @@
         <v>111.70832858288136</v>
       </c>
       <c r="R65" s="45" t="n">
-        <v>0.013</v>
+        <v>0.014</v>
       </c>
     </row>
     <row r="66">
@@ -5794,7 +6067,7 @@
         <v>104.34379289732405</v>
       </c>
       <c r="R67" s="45" t="n">
-        <v>0.015</v>
+        <v>0.021</v>
       </c>
     </row>
     <row r="68">
@@ -5852,7 +6125,7 @@
         <v>140.4656198011365</v>
       </c>
       <c r="R68" s="45" t="n">
-        <v>0.009</v>
+        <v>0.055</v>
       </c>
     </row>
     <row r="69">
@@ -5910,7 +6183,7 @@
         <v>132.50090567781749</v>
       </c>
       <c r="R69" s="45" t="n">
-        <v>0.01</v>
+        <v>0.009</v>
       </c>
     </row>
     <row r="70">
@@ -5968,7 +6241,7 @@
         <v>118.81585552012493</v>
       </c>
       <c r="R70" s="45" t="n">
-        <v>0.011</v>
+        <v>0.013</v>
       </c>
     </row>
     <row r="71">
@@ -6026,7 +6299,7 @@
         <v>103.03940834854043</v>
       </c>
       <c r="R71" s="45" t="n">
-        <v>0.017</v>
+        <v>0.015</v>
       </c>
     </row>
     <row r="72">
@@ -6084,7 +6357,7 @@
         <v>131.19036647187858</v>
       </c>
       <c r="R72" s="45" t="n">
-        <v>0.01</v>
+        <v>0.014</v>
       </c>
     </row>
     <row r="73">
@@ -6142,7 +6415,7 @@
         <v>151.60914856804686</v>
       </c>
       <c r="R73" s="45" t="n">
-        <v>0.01</v>
+        <v>0.011</v>
       </c>
     </row>
     <row r="74">
@@ -6200,7 +6473,7 @@
         <v>221.0</v>
       </c>
       <c r="R74" s="45" t="n">
-        <v>0.006</v>
+        <v>0.007</v>
       </c>
     </row>
     <row r="75">
@@ -6432,7 +6705,7 @@
         <v>221.0</v>
       </c>
       <c r="R78" s="45" t="n">
-        <v>0.009</v>
+        <v>0.055</v>
       </c>
     </row>
     <row r="79">
@@ -6490,7 +6763,7 @@
         <v>221.0</v>
       </c>
       <c r="R79" s="45" t="n">
-        <v>0.008</v>
+        <v>0.009</v>
       </c>
     </row>
     <row r="80">
@@ -6548,7 +6821,7 @@
         <v>221.0</v>
       </c>
       <c r="R80" s="45" t="n">
-        <v>0.011</v>
+        <v>0.055</v>
       </c>
     </row>
     <row r="81">
@@ -6606,7 +6879,7 @@
         <v>161.62483034513423</v>
       </c>
       <c r="R81" s="45" t="n">
-        <v>0.058</v>
+        <v>0.053</v>
       </c>
     </row>
     <row r="82">
@@ -6664,7 +6937,7 @@
         <v>149.5981155846649</v>
       </c>
       <c r="R82" s="45" t="n">
-        <v>0.019</v>
+        <v>0.015</v>
       </c>
     </row>
     <row r="83">
@@ -6722,7 +6995,7 @@
         <v>221.0</v>
       </c>
       <c r="R83" s="45" t="n">
-        <v>0.05</v>
+        <v>0.007</v>
       </c>
     </row>
     <row r="84">
@@ -6780,7 +7053,7 @@
         <v>221.0</v>
       </c>
       <c r="R84" s="45" t="n">
-        <v>0.007</v>
+        <v>0.011</v>
       </c>
     </row>
     <row r="85">
@@ -6838,7 +7111,7 @@
         <v>107.62988220575821</v>
       </c>
       <c r="R85" s="45" t="n">
-        <v>0.014</v>
+        <v>0.013</v>
       </c>
     </row>
     <row r="86">
@@ -6896,7 +7169,7 @@
         <v>102.30829706722372</v>
       </c>
       <c r="R86" s="45" t="n">
-        <v>0.016</v>
+        <v>0.017</v>
       </c>
     </row>
     <row r="87">
@@ -6954,7 +7227,7 @@
         <v>99.66960507086627</v>
       </c>
       <c r="R87" s="45" t="n">
-        <v>0.018</v>
+        <v>0.062</v>
       </c>
     </row>
     <row r="88">
@@ -7012,7 +7285,7 @@
         <v>109.4556547663558</v>
       </c>
       <c r="R88" s="45" t="n">
-        <v>0.008</v>
+        <v>0.009</v>
       </c>
     </row>
     <row r="89">
@@ -7128,7 +7401,7 @@
         <v>221.0</v>
       </c>
       <c r="R90" s="45" t="n">
-        <v>0.007</v>
+        <v>0.006</v>
       </c>
     </row>
     <row r="91">
@@ -7186,7 +7459,7 @@
         <v>107.02716095647355</v>
       </c>
       <c r="R91" s="45" t="n">
-        <v>0.027</v>
+        <v>0.008</v>
       </c>
     </row>
     <row r="92">
@@ -7360,7 +7633,7 @@
         <v>120.61229183183235</v>
       </c>
       <c r="R94" s="45" t="n">
-        <v>0.009</v>
+        <v>0.007</v>
       </c>
     </row>
     <row r="95">
@@ -7476,7 +7749,7 @@
         <v>109.00889335133512</v>
       </c>
       <c r="R96" s="45" t="n">
-        <v>0.011</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="97">
@@ -7534,7 +7807,7 @@
         <v>118.37999486566261</v>
       </c>
       <c r="R97" s="45" t="n">
-        <v>0.011</v>
+        <v>0.009</v>
       </c>
     </row>
     <row r="98">
@@ -7592,7 +7865,7 @@
         <v>104.44372932126763</v>
       </c>
       <c r="R98" s="45" t="n">
-        <v>0.053</v>
+        <v>0.058</v>
       </c>
     </row>
     <row r="99">
@@ -7650,7 +7923,7 @@
         <v>165.8443791670323</v>
       </c>
       <c r="R99" s="45" t="n">
-        <v>0.01</v>
+        <v>0.008</v>
       </c>
     </row>
     <row r="100">
@@ -7824,7 +8097,7 @@
         <v>115.5196055428162</v>
       </c>
       <c r="R102" s="45" t="n">
-        <v>0.008</v>
+        <v>0.006</v>
       </c>
     </row>
     <row r="103">
@@ -7998,7 +8271,7 @@
         <v>#NUM!</v>
       </c>
       <c r="R105" s="45" t="n">
-        <v>0.005</v>
+        <v>0.004</v>
       </c>
     </row>
     <row r="106">
@@ -8056,7 +8329,7 @@
         <v>142.71816866484232</v>
       </c>
       <c r="R106" s="45" t="n">
-        <v>0.007</v>
+        <v>0.006</v>
       </c>
     </row>
     <row r="107">
@@ -8114,7 +8387,7 @@
         <v>145.42961948150045</v>
       </c>
       <c r="R107" s="45" t="n">
-        <v>0.007</v>
+        <v>0.008</v>
       </c>
     </row>
     <row r="108">
@@ -8172,7 +8445,7 @@
         <v>221.0</v>
       </c>
       <c r="R108" s="45" t="n">
-        <v>1.9</v>
+        <v>1.935</v>
       </c>
     </row>
     <row r="109">
@@ -8288,7 +8561,7 @@
         <v>114.54162457205497</v>
       </c>
       <c r="R110" s="45" t="n">
-        <v>0.009</v>
+        <v>0.008</v>
       </c>
     </row>
     <row r="111">
@@ -8636,7 +8909,7 @@
         <v>100.54502911827619</v>
       </c>
       <c r="R116" s="45" t="n">
-        <v>0.012</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="117">
@@ -8752,7 +9025,7 @@
         <v>110.41661207537933</v>
       </c>
       <c r="R118" s="45" t="n">
-        <v>0.02</v>
+        <v>0.008</v>
       </c>
     </row>
     <row r="119">
@@ -8810,7 +9083,7 @@
         <v>105.26154228636585</v>
       </c>
       <c r="R119" s="45" t="n">
-        <v>0.017</v>
+        <v>0.016</v>
       </c>
     </row>
     <row r="120">
@@ -8868,7 +9141,7 @@
         <v>137.3171307364425</v>
       </c>
       <c r="R120" s="45" t="n">
-        <v>0.061</v>
+        <v>0.057</v>
       </c>
     </row>
     <row r="121">
@@ -8926,7 +9199,7 @@
         <v>117.63573797074517</v>
       </c>
       <c r="R121" s="45" t="n">
-        <v>0.012</v>
+        <v>0.054</v>
       </c>
     </row>
     <row r="122">
@@ -8984,7 +9257,7 @@
         <v>#NUM!</v>
       </c>
       <c r="R122" s="45" t="n">
-        <v>0.005</v>
+        <v>0.006</v>
       </c>
     </row>
     <row r="123">

</xml_diff>